<commit_message>
Finalisation du passage en revue des cas de tests problématiques
</commit_message>
<xml_diff>
--- a/scripts/043/tableau_cas_de_tests.xlsx
+++ b/scripts/043/tableau_cas_de_tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="28515" windowHeight="11325"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="28515" windowHeight="11325" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1104" uniqueCount="587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="592">
   <si>
     <t>zone</t>
   </si>
@@ -1777,6 +1777,21 @@
   </si>
   <si>
     <t>La notice a déjà une 043    $o ba</t>
+  </si>
+  <si>
+    <t>Specs pas claires : on a actuellement une 043 $o ic $b de, que les specs demandent de remplacer par une 043 $o ic --&gt; la 043 $b de a disparu. Faut-il la garder ? Ou seulement le temps des traitements ?</t>
+  </si>
+  <si>
+    <t>Specs pas claires : on a actuellement une 043 $o ic $b es, que les specs demandent de remplacer par une 043 $o ic --&gt; la 043 $b es a disparu. Faut-il la garder ? Ou seulement le temps des traitements ?</t>
+  </si>
+  <si>
+    <t>Specs pas claires : on a actuellement une 043 $o ic $b ph, que les specs demandent de remplacer par une 043 $o ic --&gt; la 043 $b ph a disparu. Faut-il la garder ? Ou seulement le temps des traitements ?</t>
+  </si>
+  <si>
+    <t>Il y a une 043 $o te au lieu de 043 $o mi --&gt; les règles d'injection de la 065 ne sont pas appliquées</t>
+  </si>
+  <si>
+    <t>Il y a une 043 $o ic au lieu de 043 $o mi --&gt; les règles d'injection de la 065 ne sont pas appliquées</t>
   </si>
 </sst>
 </file>
@@ -2140,10 +2155,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F160"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A125" workbookViewId="0">
-      <selection sqref="A1:F156"/>
+    <sheetView topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="A127" sqref="A127:E127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4352,55 +4367,55 @@
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="F123" s="2"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="F124" s="2"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>395</v>
+        <v>407</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>396</v>
+        <v>408</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>397</v>
+        <v>409</v>
       </c>
       <c r="F125" s="2"/>
     </row>
@@ -4412,211 +4427,176 @@
         <v>6</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>398</v>
+        <v>419</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>399</v>
+        <v>420</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>400</v>
+        <v>421</v>
       </c>
       <c r="F126" s="2"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="B127" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C127" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="D127" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="E127" s="1" t="s">
-        <v>403</v>
-      </c>
       <c r="F127" s="2"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>405</v>
-      </c>
+        <v>433</v>
+      </c>
+      <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
-        <v>406</v>
+        <v>434</v>
       </c>
       <c r="F128" s="2"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>408</v>
-      </c>
+        <v>435</v>
+      </c>
+      <c r="D129" s="1"/>
       <c r="E129" s="1" t="s">
-        <v>409</v>
+        <v>436</v>
       </c>
       <c r="F129" s="2"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="D130" s="1" t="s">
-        <v>411</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="D130" s="1"/>
       <c r="E130" s="1" t="s">
-        <v>412</v>
+        <v>438</v>
       </c>
       <c r="F130" s="2"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="D131" s="1" t="s">
-        <v>414</v>
-      </c>
+        <v>439</v>
+      </c>
+      <c r="D131" s="1"/>
       <c r="E131" s="1" t="s">
-        <v>415</v>
+        <v>440</v>
       </c>
       <c r="F131" s="2"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>417</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="D132" s="1"/>
       <c r="E132" s="1" t="s">
-        <v>418</v>
+        <v>441</v>
       </c>
       <c r="F132" s="2"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>419</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>420</v>
-      </c>
+        <v>442</v>
+      </c>
+      <c r="D133" s="1"/>
       <c r="E133" s="1" t="s">
-        <v>421</v>
+        <v>443</v>
       </c>
       <c r="F133" s="2"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="D134" s="1" t="s">
-        <v>423</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="D134" s="1"/>
       <c r="E134" s="1" t="s">
-        <v>424</v>
+        <v>444</v>
       </c>
       <c r="F134" s="2"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>426</v>
-      </c>
+        <v>445</v>
+      </c>
+      <c r="D135" s="1"/>
       <c r="E135" s="1" t="s">
-        <v>427</v>
+        <v>446</v>
       </c>
       <c r="F135" s="2"/>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>429</v>
-      </c>
+        <v>445</v>
+      </c>
+      <c r="D136" s="1"/>
       <c r="E136" s="1" t="s">
-        <v>430</v>
+        <v>447</v>
       </c>
       <c r="F136" s="2"/>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>6</v>
+        <v>432</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>399</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="D137" s="1"/>
       <c r="E137" s="1" t="s">
-        <v>431</v>
+        <v>450</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -4628,11 +4608,11 @@
         <v>432</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>433</v>
+        <v>439</v>
       </c>
       <c r="D138" s="1"/>
       <c r="E138" s="1" t="s">
-        <v>434</v>
+        <v>451</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -4644,11 +4624,11 @@
         <v>432</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1" t="s">
-        <v>436</v>
+        <v>452</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -4660,11 +4640,11 @@
         <v>432</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1" t="s">
-        <v>438</v>
+        <v>453</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -4676,11 +4656,11 @@
         <v>432</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1" t="s">
-        <v>440</v>
+        <v>454</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -4696,7 +4676,7 @@
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1" t="s">
-        <v>441</v>
+        <v>455</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -4712,7 +4692,7 @@
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1" t="s">
-        <v>443</v>
+        <v>456</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -4724,11 +4704,11 @@
         <v>432</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1" t="s">
-        <v>444</v>
+        <v>457</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -4740,11 +4720,11 @@
         <v>432</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1" t="s">
-        <v>446</v>
+        <v>458</v>
       </c>
       <c r="F145" s="2"/>
     </row>
@@ -4756,185 +4736,46 @@
         <v>432</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>445</v>
+        <v>437</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1" t="s">
-        <v>447</v>
+        <v>231</v>
       </c>
       <c r="F146" s="2"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B147" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>448</v>
-      </c>
-      <c r="D147" s="1"/>
-      <c r="E147" s="1" t="s">
-        <v>450</v>
-      </c>
       <c r="F147" s="2"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B148" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D148" s="1"/>
-      <c r="E148" s="1" t="s">
-        <v>451</v>
-      </c>
       <c r="F148" s="2"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B149" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="D149" s="1"/>
-      <c r="E149" s="1" t="s">
-        <v>452</v>
-      </c>
       <c r="F149" s="2"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B150" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D150" s="1"/>
-      <c r="E150" s="1" t="s">
-        <v>453</v>
-      </c>
       <c r="F150" s="2"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B151" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="D151" s="1"/>
-      <c r="E151" s="1" t="s">
-        <v>454</v>
-      </c>
       <c r="F151" s="2"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="D152" s="1"/>
-      <c r="E152" s="1" t="s">
-        <v>455</v>
-      </c>
       <c r="F152" s="2"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="D153" s="1"/>
-      <c r="E153" s="1" t="s">
-        <v>456</v>
-      </c>
       <c r="F153" s="2"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="D154" s="1"/>
-      <c r="E154" s="1" t="s">
-        <v>457</v>
-      </c>
       <c r="F154" s="2"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="D155" s="1"/>
-      <c r="E155" s="1" t="s">
-        <v>458</v>
-      </c>
       <c r="F155" s="2"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="D156" s="1"/>
-      <c r="E156" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="F156" s="2"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F157" s="2"/>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F158" s="2"/>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F159" s="2"/>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F160" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4944,10 +4785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F57"/>
+  <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45:F57"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6086,6 +5927,226 @@
       </c>
       <c r="F57" s="5" t="s">
         <v>585</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>578</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>590</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif extension cas de tests
</commit_message>
<xml_diff>
--- a/scripts/043/tableau_cas_de_tests.xlsx
+++ b/scripts/043/tableau_cas_de_tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="28515" windowHeight="11325" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="135" windowWidth="28515" windowHeight="11325"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2157,8 +2157,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F157"/>
   <sheetViews>
-    <sheetView topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="A127" sqref="A127:E127"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection sqref="A1:F145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4438,6 +4438,19 @@
       <c r="F126" s="2"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D127" s="1"/>
+      <c r="E127" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="F127" s="2"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -4448,11 +4461,11 @@
         <v>432</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D128" s="1"/>
       <c r="E128" s="1" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="F128" s="2"/>
     </row>
@@ -4464,11 +4477,11 @@
         <v>432</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="D129" s="1"/>
       <c r="E129" s="1" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="F129" s="2"/>
     </row>
@@ -4480,11 +4493,11 @@
         <v>432</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D130" s="1"/>
       <c r="E130" s="1" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="F130" s="2"/>
     </row>
@@ -4496,11 +4509,11 @@
         <v>432</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>439</v>
+        <v>328</v>
       </c>
       <c r="D131" s="1"/>
       <c r="E131" s="1" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="F131" s="2"/>
     </row>
@@ -4512,11 +4525,11 @@
         <v>432</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>328</v>
+        <v>442</v>
       </c>
       <c r="D132" s="1"/>
       <c r="E132" s="1" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="F132" s="2"/>
     </row>
@@ -4528,11 +4541,11 @@
         <v>432</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="F133" s="2"/>
     </row>
@@ -4544,11 +4557,11 @@
         <v>432</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>437</v>
+        <v>445</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="F134" s="2"/>
     </row>
@@ -4564,7 +4577,7 @@
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F135" s="2"/>
     </row>
@@ -4576,11 +4589,11 @@
         <v>432</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="F136" s="2"/>
     </row>
@@ -4592,11 +4605,11 @@
         <v>432</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F137" s="2"/>
     </row>
@@ -4608,11 +4621,11 @@
         <v>432</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D138" s="1"/>
       <c r="E138" s="1" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F138" s="2"/>
     </row>
@@ -4624,11 +4637,11 @@
         <v>432</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="F139" s="2"/>
     </row>
@@ -4640,11 +4653,11 @@
         <v>432</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="F140" s="2"/>
     </row>
@@ -4656,11 +4669,11 @@
         <v>432</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>437</v>
+        <v>328</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="F141" s="2"/>
     </row>
@@ -4672,11 +4685,11 @@
         <v>432</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>328</v>
+        <v>442</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F142" s="2"/>
     </row>
@@ -4688,11 +4701,11 @@
         <v>432</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="F143" s="2"/>
     </row>
@@ -4704,11 +4717,11 @@
         <v>432</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="D144" s="1"/>
       <c r="E144" s="1" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F144" s="2"/>
     </row>
@@ -4720,28 +4733,15 @@
         <v>432</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1" t="s">
-        <v>458</v>
+        <v>231</v>
       </c>
       <c r="F145" s="2"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="B146" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="D146" s="1"/>
-      <c r="E146" s="1" t="s">
-        <v>231</v>
-      </c>
       <c r="F146" s="2"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.25">
@@ -4787,7 +4787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>

</xml_diff>